<commit_message>
updated BOM, completed Layout. Still need to add team number and project description to schematic
</commit_message>
<xml_diff>
--- a/Documents/ECE_411_Bill_of_Materials.xlsx
+++ b/Documents/ECE_411_Bill_of_Materials.xlsx
@@ -1,18 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshd\Documents\Josh's\College\PSU!\ECE 411 Industry Design Processes\ece411\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B88C9AC-60E9-4248-B36C-0B6BE852CAB2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
   <si>
     <t>Table 1</t>
   </si>
@@ -107,9 +122,6 @@
     <t>C12</t>
   </si>
   <si>
-    <t>10uf</t>
-  </si>
-  <si>
     <t>UWT1V100MCL1GB</t>
   </si>
   <si>
@@ -140,24 +152,12 @@
     <t>AVR ISP HEADER</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>0473460001_USBMICRO</t>
-  </si>
-  <si>
     <t>MOLEX_USBMICRO</t>
   </si>
   <si>
-    <t>USB Micro Connector</t>
-  </si>
-  <si>
     <t>LED1, LED2</t>
   </si>
   <si>
-    <t>LEDSMT1206</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -218,9 +218,6 @@
     <t>TQFP44</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>ATS160SM-1</t>
   </si>
   <si>
@@ -252,15 +249,102 @@
   </si>
   <si>
     <t>Total $:</t>
+  </si>
+  <si>
+    <t>XTAL1</t>
+  </si>
+  <si>
+    <t>047346-0001</t>
+  </si>
+  <si>
+    <t>MICRO_USB</t>
+  </si>
+  <si>
+    <t>USB Micro Connector Type B</t>
+  </si>
+  <si>
+    <t>QBLP650-AG</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>DC Barrel Jack (Thru-Hole)</t>
+  </si>
+  <si>
+    <t>Dielectric (Polarized) Capacitor</t>
+  </si>
+  <si>
+    <t>Push Button SPST Switch N.O.</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>Crystal Oscillator</t>
+  </si>
+  <si>
+    <t>MFG</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>QT-Brightek</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>Nichicon</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>KOA Speer Electronics</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>KEMET Corp</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>CTS</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Servo Motor</t>
+  </si>
+  <si>
+    <t>SG90</t>
+  </si>
+  <si>
+    <t>PINHD-1X3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -273,7 +357,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -414,73 +498,73 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,26 +574,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -708,7 +851,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -727,7 +870,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -757,7 +900,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -783,7 +926,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -809,7 +952,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -835,7 +978,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -861,7 +1004,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -887,7 +1030,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -913,7 +1056,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -939,7 +1082,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -965,7 +1108,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -978,9 +1121,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -997,7 +1146,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1016,7 +1165,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1042,7 +1191,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1068,7 +1217,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1094,7 +1243,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1120,7 +1269,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1146,7 +1295,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1172,7 +1321,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1198,7 +1347,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1224,7 +1373,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1250,7 +1399,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,9 +1412,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1279,7 +1434,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1298,7 +1453,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1328,7 +1483,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1354,7 +1509,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1380,7 +1535,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1406,7 +1561,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1432,7 +1587,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1458,7 +1613,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1484,7 +1639,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1510,7 +1665,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1536,7 +1691,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1549,645 +1704,801 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I23"/>
+  <dimension ref="A1:IX24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.1719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="30" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6719" style="1" customWidth="1"/>
-    <col min="10" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="7" max="9" width="12.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
+    <col min="12" max="258" width="8.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:11" ht="27.6" customHeight="1">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4">
+    <row r="3" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" t="s" s="7">
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s" s="7">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9">
+      <c r="G3" s="7"/>
+      <c r="H3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8">
         <v>0.52</v>
       </c>
-      <c r="I3" s="9">
+      <c r="K3" s="8">
         <v>0.52</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="10">
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s" s="12">
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="13">
+      <c r="D4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s" s="13">
+      <c r="E4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s" s="13">
+      <c r="F4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s" s="13">
+      <c r="G4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="13">
         <v>0.34</v>
       </c>
-      <c r="I4" s="14">
+      <c r="K4" s="13">
         <v>0.34</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="10">
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="9">
         <v>6</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s" s="12">
+      <c r="C5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s" s="13">
+      <c r="E5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s" s="13">
+      <c r="F5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s" s="13">
+      <c r="G5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="13">
         <v>0.41</v>
       </c>
-      <c r="I5" s="14">
+      <c r="K5" s="13">
         <v>2.46</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="10">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" t="s" s="11">
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s" s="12">
+      <c r="C6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s" s="13">
+      <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s" s="13">
+      <c r="E6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s" s="13">
+      <c r="F6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s" s="13">
+      <c r="G6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="14">
-        <v>0.0125</v>
-      </c>
-      <c r="I6" s="14">
-        <v>0.025</v>
+      <c r="H6" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="K6" s="13">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="10">
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s" s="12">
+      <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s" s="13">
+      <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s" s="13">
+      <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s" s="13">
+      <c r="F7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="s" s="13">
+      <c r="G7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="13">
         <v>0.5</v>
       </c>
-      <c r="I7" s="14">
+      <c r="K7" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="10">
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="9">
         <v>1</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s" s="12">
+      <c r="C8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s" s="13">
+      <c r="E8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E8" t="s" s="13">
+      <c r="F8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.04</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" t="s" s="13">
+      <c r="C9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="14">
-        <v>0.04</v>
-      </c>
-      <c r="I8" s="14">
-        <v>0.04</v>
+      <c r="H9" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0.32</v>
+      </c>
+      <c r="K9" s="13">
+        <v>0.32</v>
       </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="10">
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B9" t="s" s="11">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s" s="12">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s" s="13">
+      <c r="B10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G9" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="H9" s="14">
-        <v>0.32</v>
-      </c>
-      <c r="I9" s="14">
-        <v>0.32</v>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0.52</v>
       </c>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="10">
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="9">
         <v>1</v>
       </c>
-      <c r="B10" t="s" s="11">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s" s="12">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s" s="13">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s" s="13">
+      <c r="B11" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14">
+      <c r="F11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="9">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1206</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0.34</v>
+      </c>
+      <c r="K12" s="13">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="9">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="16">
+        <v>22</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.21</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="9">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0.09</v>
+      </c>
+      <c r="K14" s="13">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="9">
+        <v>1</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0.21</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="9">
+        <v>2</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="K16" s="13">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="9">
+        <v>2</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="9">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="13">
         <v>0.52</v>
       </c>
-      <c r="I10" s="14">
+      <c r="K18" s="13">
         <v>0.52</v>
       </c>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="10">
+    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="9">
         <v>1</v>
       </c>
-      <c r="B11" t="s" s="11">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s" s="12">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s" s="13">
-        <v>43</v>
-      </c>
-      <c r="E11" t="s" s="13">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s" s="13">
-        <v>45</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="14">
-        <v>0.598</v>
-      </c>
-      <c r="I11" s="14">
-        <v>0.598</v>
+      <c r="B19" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="13">
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="K19" s="13">
+        <v>3.9550000000000001</v>
       </c>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="10">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s" s="11">
-        <v>46</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" t="s" s="13">
-        <v>47</v>
-      </c>
-      <c r="E12" s="14">
-        <v>1206</v>
-      </c>
-      <c r="F12" t="s" s="13">
-        <v>48</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="14">
-        <v>0.34</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0.68</v>
+    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="9">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J20" s="13">
+        <v>0.27</v>
+      </c>
+      <c r="K20" s="13">
+        <v>0.27</v>
       </c>
     </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="10">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s" s="11">
-        <v>49</v>
-      </c>
-      <c r="C13" s="17">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s" s="13">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s" s="13">
-        <v>51</v>
-      </c>
-      <c r="F13" t="s" s="13">
-        <v>52</v>
-      </c>
-      <c r="G13" t="s" s="13">
-        <v>53</v>
-      </c>
-      <c r="H13" s="14">
-        <v>0.21</v>
-      </c>
-      <c r="I13" s="14">
-        <v>0.42</v>
+    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="9">
+        <v>1</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" s="13">
+        <v>1.9</v>
+      </c>
+      <c r="K21" s="13">
+        <v>1.9</v>
       </c>
     </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="10">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s" s="11">
-        <v>54</v>
-      </c>
-      <c r="C14" t="s" s="12">
-        <v>55</v>
-      </c>
-      <c r="D14" t="s" s="13">
-        <v>56</v>
-      </c>
-      <c r="E14" t="s" s="13">
-        <v>51</v>
-      </c>
-      <c r="F14" t="s" s="13">
-        <v>52</v>
-      </c>
-      <c r="G14" t="s" s="13">
-        <v>53</v>
-      </c>
-      <c r="H14" s="14">
-        <v>0.09</v>
-      </c>
-      <c r="I14" s="14">
-        <v>0.18</v>
+    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="9">
+        <v>1</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="10">
+    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="9">
         <v>1</v>
       </c>
-      <c r="B15" t="s" s="11">
-        <v>57</v>
-      </c>
-      <c r="C15" t="s" s="12">
-        <v>58</v>
-      </c>
-      <c r="D15" t="s" s="13">
-        <v>59</v>
-      </c>
-      <c r="E15" t="s" s="13">
-        <v>51</v>
-      </c>
-      <c r="F15" t="s" s="13">
-        <v>52</v>
-      </c>
-      <c r="G15" t="s" s="13">
-        <v>53</v>
-      </c>
-      <c r="H15" s="14">
-        <v>0.21</v>
-      </c>
-      <c r="I15" s="14">
-        <v>0.21</v>
+      <c r="B23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="13">
+        <v>2.15</v>
+      </c>
+      <c r="K23" s="13">
+        <v>2.15</v>
       </c>
     </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="10">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s" s="11">
-        <v>60</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" t="s" s="13">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="F16" t="s" s="13">
-        <v>13</v>
-      </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="14">
-        <v>1.8</v>
-      </c>
-      <c r="I16" s="14">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="10">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s" s="11">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s" s="12">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s" s="13">
-        <v>64</v>
-      </c>
-      <c r="E17" t="s" s="13">
-        <v>64</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="14">
-        <v>0.52</v>
-      </c>
-      <c r="I17" s="14">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s" s="11">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s" s="12">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s" s="13">
-        <v>66</v>
-      </c>
-      <c r="E18" t="s" s="13">
-        <v>67</v>
-      </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="14">
-        <v>3.955</v>
-      </c>
-      <c r="I18" s="14">
-        <v>3.955</v>
-      </c>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="10">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s" s="11">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s" s="12">
-        <v>69</v>
-      </c>
-      <c r="D19" t="s" s="13">
-        <v>69</v>
-      </c>
-      <c r="E19" t="s" s="13">
-        <v>69</v>
-      </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14">
-        <v>0.27</v>
-      </c>
-      <c r="I19" s="14">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="10">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s" s="11">
-        <v>70</v>
-      </c>
-      <c r="C20" t="s" s="12">
-        <v>71</v>
-      </c>
-      <c r="D20" t="s" s="13">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="F20" t="s" s="13">
+    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="14">
-        <v>1.9</v>
-      </c>
-      <c r="I20" s="14">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="10">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s" s="11">
-        <v>74</v>
-      </c>
-      <c r="C21" t="s" s="12">
-        <v>75</v>
-      </c>
-      <c r="D21" t="s" s="13">
-        <v>75</v>
-      </c>
-      <c r="E21" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="F21" t="s" s="13">
-        <v>76</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="14">
-        <v>0.55</v>
-      </c>
-      <c r="I21" s="14">
-        <v>0.55</v>
-      </c>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="10">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s" s="11">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s" s="12">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s" s="13">
-        <v>78</v>
-      </c>
-      <c r="E22" t="s" s="13">
-        <v>78</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="14">
-        <v>2.15</v>
-      </c>
-      <c r="I22" s="14">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" t="s" s="20">
-        <v>79</v>
-      </c>
-      <c r="I23" s="14">
-        <f>SUM(I3:I22)</f>
-        <v>20.258</v>
+      <c r="K24" s="13">
+        <f>SUM(K3:K23)</f>
+        <v>20.257999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
updated the BOM excel
</commit_message>
<xml_diff>
--- a/Documents/ECE_411_Bill_of_Materials.xlsx
+++ b/Documents/ECE_411_Bill_of_Materials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshd\Documents\Josh's\College\PSU!\ECE 411 Industry Design Processes\ece411\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshd\Documents\Josh's\College\PSU!\ECE 411 Industry Design Processes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B88C9AC-60E9-4248-B36C-0B6BE852CAB2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4499ED49-5C0D-444B-BC7B-DAEE559BF41D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>Table 1</t>
   </si>
@@ -116,9 +116,6 @@
     <t>10u</t>
   </si>
   <si>
-    <t>CL31A106KOCLNNC</t>
-  </si>
-  <si>
     <t>C12</t>
   </si>
   <si>
@@ -339,6 +336,15 @@
   </si>
   <si>
     <t>PINHD-1X3</t>
+  </si>
+  <si>
+    <t>CL31A106MOHNNNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost ext. </t>
+  </si>
+  <si>
+    <t>3462</t>
   </si>
 </sst>
 </file>
@@ -502,7 +508,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -551,9 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -561,6 +564,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1726,42 +1735,46 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IX24"/>
+  <dimension ref="A1:IY24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30" style="1" customWidth="1"/>
-    <col min="7" max="9" width="12.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
-    <col min="12" max="258" width="8.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="259" width="8.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27.6" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:12" ht="27.6" customHeight="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:11" ht="20.25" customHeight="1">
+    <row r="2" spans="1:12" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1784,19 +1797,22 @@
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="20.25" customHeight="1">
+    <row r="3" spans="1:12" ht="20.25" customHeight="1">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1815,17 +1831,21 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="8">
         <v>0.52</v>
       </c>
       <c r="K3" s="8">
+        <f>J3*A3</f>
         <v>0.52</v>
       </c>
+      <c r="L3" s="8">
+        <v>0.52</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1848,19 +1868,23 @@
         <v>19</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J4" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="K4" s="13">
+        <f>J4*A4</f>
+        <v>0.52</v>
+      </c>
+      <c r="L4" s="13">
         <v>0.34</v>
       </c>
-      <c r="K4" s="13">
-        <v>0.34</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="9">
         <v>6</v>
       </c>
@@ -1883,19 +1907,23 @@
         <v>19</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J5" s="13">
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
       <c r="K5" s="13">
+        <f t="shared" ref="K5:K23" si="0">J5*A5</f>
+        <v>2.64</v>
+      </c>
+      <c r="L5" s="13">
         <v>2.46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="9">
         <v>2</v>
       </c>
@@ -1918,19 +1946,23 @@
         <v>19</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="13">
-        <v>1.2500000000000001E-2</v>
+        <v>0.27</v>
       </c>
       <c r="K6" s="13">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="L6" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>27</v>
@@ -1939,7 +1971,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>17</v>
@@ -1951,533 +1983,601 @@
         <v>19</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J7" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="K7" s="13">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K7" s="13">
+      <c r="L7" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="9">
         <v>1</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J8" s="13">
         <v>0.04</v>
       </c>
       <c r="K8" s="13">
+        <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
+      <c r="L8" s="13">
+        <v>0.04</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="9">
         <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J9" s="13">
+        <v>0.33</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="L9" s="13">
         <v>0.32</v>
       </c>
-      <c r="K9" s="13">
-        <v>0.32</v>
-      </c>
     </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="13">
         <v>0.52</v>
       </c>
       <c r="K10" s="13">
+        <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
+      <c r="L10" s="13">
+        <v>0.52</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="9">
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J11" s="13">
         <v>0.59799999999999998</v>
       </c>
       <c r="K11" s="13">
+        <f t="shared" si="0"/>
         <v>0.59799999999999998</v>
       </c>
+      <c r="L11" s="13">
+        <v>0.59799999999999998</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="9">
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" s="13">
         <v>1206</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="14" t="s">
-        <v>88</v>
-      </c>
       <c r="J12" s="13">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="K12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+      <c r="L12" s="13">
         <v>0.68</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="9">
         <v>2</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="19">
+        <v>22</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="16">
-        <v>22</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="F13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="G13" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>48</v>
-      </c>
       <c r="H13" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J13" s="13">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="K13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.44</v>
+      </c>
+      <c r="L13" s="13">
         <v>0.42</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="9">
         <v>2</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="E14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>48</v>
-      </c>
       <c r="H14" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J14" s="13">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="K14" s="13">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="L14" s="13">
         <v>0.18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="9">
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>54</v>
-      </c>
       <c r="E15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="G15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>48</v>
-      </c>
       <c r="H15" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J15" s="13">
+        <v>0.22</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="L15" s="13">
         <v>0.21</v>
       </c>
-      <c r="K15" s="13">
-        <v>0.21</v>
-      </c>
     </row>
-    <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="9">
         <v>2</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="13">
         <v>1.8</v>
       </c>
       <c r="K16" s="13">
+        <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
+      <c r="L16" s="13">
+        <v>3.6</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="9">
         <v>2</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="K17" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="9">
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J18" s="13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L18" s="13">
         <v>0.52</v>
       </c>
-      <c r="K18" s="13">
-        <v>0.52</v>
-      </c>
     </row>
-    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="9">
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="F19" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="13">
         <v>3.9550000000000001</v>
       </c>
       <c r="K19" s="13">
+        <f t="shared" si="0"/>
         <v>3.9550000000000001</v>
       </c>
+      <c r="L19" s="13">
+        <v>3.9550000000000001</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="9">
         <v>1</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J20" s="13">
+        <v>0.32</v>
+      </c>
+      <c r="K20" s="13">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="L20" s="13">
         <v>0.27</v>
       </c>
-      <c r="K20" s="13">
-        <v>0.27</v>
-      </c>
     </row>
-    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="9">
         <v>1</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J21" s="13">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K21" s="13">
+        <f t="shared" si="0"/>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="L21" s="13">
         <v>1.9</v>
       </c>
-      <c r="K21" s="13">
-        <v>1.9</v>
-      </c>
     </row>
-    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="9">
         <v>1</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>70</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J22" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="K22" s="13">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="L22" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K22" s="13">
-        <v>0.55000000000000004</v>
-      </c>
     </row>
-    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="9">
         <v>1</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>72</v>
-      </c>
       <c r="D23" s="12" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J23" s="13">
         <v>2.15</v>
       </c>
       <c r="K23" s="13">
+        <f t="shared" si="0"/>
         <v>2.15</v>
       </c>
+      <c r="L23" s="13">
+        <v>2.15</v>
+      </c>
     </row>
-    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
+    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="15"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -2485,17 +2585,21 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
-      <c r="J24" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="K24" s="13">
+      <c r="J24" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K24" s="20">
         <f>SUM(K3:K23)</f>
+        <v>21.163</v>
+      </c>
+      <c r="L24" s="13">
+        <f>SUM(L3:L23)</f>
         <v>20.257999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Arrow BOM excel file, and updated our BOM excel file to include the two headers we'll order
</commit_message>
<xml_diff>
--- a/Documents/ECE_411_Bill_of_Materials.xlsx
+++ b/Documents/ECE_411_Bill_of_Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshd\Documents\Josh's\College\PSU!\ECE 411 Industry Design Processes\ece411\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742E33CA-3AB6-4D18-9654-381D674E7990}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE171FAE-D8ED-49EC-B1BC-D54D4BB76651}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="124">
   <si>
     <t>Table 1</t>
   </si>
@@ -59,15 +59,6 @@
     <t>Cost ext. ($)</t>
   </si>
   <si>
-    <t>BUTTON_PAD</t>
-  </si>
-  <si>
-    <t>PINHD-1X5</t>
-  </si>
-  <si>
-    <t>1X05</t>
-  </si>
-  <si>
     <t>PIN HEADER</t>
   </si>
   <si>
@@ -191,9 +182,6 @@
     <t xml:space="preserve">SG90 9G Nylon-Gear </t>
   </si>
   <si>
-    <t>1X03</t>
-  </si>
-  <si>
     <t>SW_RST</t>
   </si>
   <si>
@@ -329,9 +317,6 @@
     <t>SG90</t>
   </si>
   <si>
-    <t>PINHD-1X3</t>
-  </si>
-  <si>
     <t>CL31A106MOHNNNE</t>
   </si>
   <si>
@@ -390,6 +375,30 @@
   </si>
   <si>
     <t>https://www.arrow.com/en/products/08052a220jat2a/avx</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>BUTTON_PAD, SERVO1, SERVO2</t>
+  </si>
+  <si>
+    <t>PINHD-1X10</t>
+  </si>
+  <si>
+    <t>1X10</t>
+  </si>
+  <si>
+    <t>https://www.arrow.com/en/products/150-1-002-0-s-xs0-0835/mpe-garry-gmbh</t>
+  </si>
+  <si>
+    <t>MPE-Garry GmbH</t>
+  </si>
+  <si>
+    <t>Adam Tech</t>
+  </si>
+  <si>
+    <t>https://www.arrow.com/en/products/hph2-a-06-ua/adam-tech</t>
   </si>
 </sst>
 </file>
@@ -562,7 +571,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -575,9 +584,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -626,16 +632,22 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1799,10 +1811,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IX24"/>
+  <dimension ref="A1:IX23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1811,30 +1823,30 @@
     <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="1" customWidth="1"/>
     <col min="12" max="258" width="8.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.6" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1859,10 +1871,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>8</v>
@@ -1871,789 +1883,770 @@
         <v>9</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1">
+    <row r="3" spans="1:12" ht="25.5">
       <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8">
-        <v>0.52</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="G3" s="6"/>
+      <c r="H3" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="K3" s="7">
         <f>J3*A3</f>
-        <v>0.52</v>
-      </c>
-      <c r="L3" s="24"/>
+        <v>0.16</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="F4" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" s="13">
+      <c r="H4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="12">
         <v>0.52</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="12">
         <f>J4*A4</f>
         <v>0.52</v>
       </c>
-      <c r="L4" s="22" t="s">
-        <v>114</v>
+      <c r="L4" s="20" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="J5" s="13">
+      <c r="E5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="12">
         <v>0.44</v>
       </c>
-      <c r="K5" s="13">
-        <f t="shared" ref="K5:K23" si="0">J5*A5</f>
+      <c r="K5" s="12">
+        <f t="shared" ref="K5:K22" si="0">J5*A5</f>
         <v>2.64</v>
       </c>
-      <c r="L5" s="22" t="s">
-        <v>115</v>
+      <c r="L5" s="20" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13">
+      <c r="F6" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="12">
         <v>0.27</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
-      <c r="L6" s="22" t="s">
-        <v>120</v>
+      <c r="L6" s="20" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="12">
         <v>0.25</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="L7" s="22" t="s">
-        <v>113</v>
+      <c r="L7" s="20" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>1</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="J8" s="13">
+      <c r="F8" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="12">
         <v>0.04</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="L8" s="23" t="s">
-        <v>106</v>
+      <c r="L8" s="21" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="J9" s="13">
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="12">
         <v>0.33</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="12">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-      <c r="L9" s="22" t="s">
-        <v>112</v>
+      <c r="L9" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>1</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="13">
-        <v>0.52</v>
-      </c>
-      <c r="K10" s="13">
+      <c r="G10" s="13"/>
+      <c r="H10" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="12">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="K10" s="12">
         <f t="shared" si="0"/>
-        <v>0.52</v>
-      </c>
-      <c r="L10" s="24"/>
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>1</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="12" t="s">
+      <c r="B11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <v>0.59799999999999998</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="12">
         <f t="shared" si="0"/>
         <v>0.59799999999999998</v>
       </c>
-      <c r="L11" s="23" t="s">
-        <v>107</v>
+      <c r="L11" s="21" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>2</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="B12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="12">
         <v>1206</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="J12" s="13">
+      <c r="F12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="12">
         <v>0.36</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="12">
         <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
-      <c r="L12" s="23" t="s">
-        <v>108</v>
+      <c r="L12" s="21" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>2</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="18">
+        <v>22</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="19">
-        <v>22</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" s="13">
+      <c r="H13" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J13" s="12">
         <v>0.22</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="12">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
-      <c r="L13" s="22" t="s">
-        <v>111</v>
+      <c r="L13" s="20" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>2</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="J14" s="13">
+      <c r="E14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="12">
         <v>0.1</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="12">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="L14" s="23" t="s">
-        <v>109</v>
+      <c r="L14" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" s="13">
+      <c r="B15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" s="12">
         <v>0.22</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="12">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="L15" s="23" t="s">
-        <v>110</v>
+      <c r="L15" s="21" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <v>2</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="13">
+      <c r="B16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="12">
         <v>1.8</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="12">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="L16" s="24"/>
+      <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="9">
-        <v>2</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="8">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13">
+      <c r="E17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K17" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="24"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="J18" s="13">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="K18" s="13">
+      <c r="F18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="13"/>
+      <c r="J18" s="12">
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="K18" s="12">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="L18" s="22" t="s">
-        <v>118</v>
-      </c>
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="L18" s="22"/>
     </row>
     <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>1</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="14" t="s">
+      <c r="B19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="13">
-        <v>3.9550000000000001</v>
-      </c>
-      <c r="K19" s="13">
+      <c r="I19" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="12">
+        <v>0.32</v>
+      </c>
+      <c r="K19" s="12">
         <f t="shared" si="0"/>
-        <v>3.9550000000000001</v>
-      </c>
-      <c r="L19" s="24"/>
+        <v>0.32</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="B20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="J20" s="13">
-        <v>0.32</v>
-      </c>
-      <c r="K20" s="13">
+      <c r="G20" s="13"/>
+      <c r="H20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="12">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K20" s="12">
         <f t="shared" si="0"/>
-        <v>0.32</v>
-      </c>
-      <c r="L20" s="22" t="s">
-        <v>119</v>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <v>1</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="J21" s="13">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="K21" s="13">
+      <c r="G21" s="13"/>
+      <c r="H21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="K21" s="12">
         <f t="shared" si="0"/>
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="L21" s="22" t="s">
-        <v>116</v>
+        <v>0.6</v>
+      </c>
+      <c r="L21" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>1</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J22" s="13">
-        <v>0.6</v>
-      </c>
-      <c r="K22" s="13">
+      <c r="D22" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="12">
+        <v>2.15</v>
+      </c>
+      <c r="K22" s="12">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="L22" s="22" t="s">
-        <v>117</v>
+        <v>2.15</v>
+      </c>
+      <c r="L22" s="21" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="9">
-        <v>1</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="J23" s="13">
-        <v>2.15</v>
-      </c>
-      <c r="K23" s="13">
-        <f t="shared" si="0"/>
-        <v>2.15</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="K24" s="20">
-        <f>SUM(K3:K23)</f>
-        <v>21.163</v>
-      </c>
-      <c r="L24" s="24"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" s="19">
+        <f>SUM(K3:K22)</f>
+        <v>20.918000000000003</v>
+      </c>
+      <c r="L23" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L23" r:id="rId1" xr:uid="{21DE8B6F-1636-4FAE-8463-228D74264259}"/>
+    <hyperlink ref="L22" r:id="rId1" xr:uid="{21DE8B6F-1636-4FAE-8463-228D74264259}"/>
     <hyperlink ref="L8" r:id="rId2" xr:uid="{42702CC6-858F-4ED1-8AC8-1D7022B4F1AA}"/>
     <hyperlink ref="L11" r:id="rId3" display="https://www.arrow.com/en/products/47346-0001/molex" xr:uid="{64DBF0B8-E67D-4803-B4E5-7E5ED1A8E3F6}"/>
     <hyperlink ref="L12" r:id="rId4" xr:uid="{60C5A004-3579-444B-894C-B7D1BDC73074}"/>
@@ -2664,14 +2657,16 @@
     <hyperlink ref="L7" r:id="rId9" display="https://www.arrow.com/en/products/cl31a106mohnnne/samsung-electro-mechanics" xr:uid="{120B6B86-07AB-4EBE-98F2-711AEE67DDB3}"/>
     <hyperlink ref="L4" r:id="rId10" display="https://www.arrow.com/en/products/c1206x105k5recauto/kemet-corporation" xr:uid="{5F35304B-FE1A-4AF9-BCBC-321A92D36C40}"/>
     <hyperlink ref="L5" r:id="rId11" xr:uid="{FEE6CF7C-37B3-4395-916E-D2DD0C3E0E6A}"/>
-    <hyperlink ref="L21" r:id="rId12" display="https://www.arrow.com/en/products/mic29310-5.0wu/microchip-technology" xr:uid="{CDD429B9-234E-4378-BBCB-B7748E26DCA9}"/>
-    <hyperlink ref="L22" r:id="rId13" xr:uid="{DD6E462B-22D3-4BCE-8BEC-EE10845B77FE}"/>
-    <hyperlink ref="L18" r:id="rId14" display="https://www.arrow.com/en/products/fsm2jsmltr/te-connectivity" xr:uid="{94B52CE5-A70B-44A1-800C-359546489236}"/>
-    <hyperlink ref="L20" r:id="rId15" xr:uid="{962D090B-5AFA-4D2A-BBC2-A5C18F9637FA}"/>
+    <hyperlink ref="L20" r:id="rId12" display="https://www.arrow.com/en/products/mic29310-5.0wu/microchip-technology" xr:uid="{CDD429B9-234E-4378-BBCB-B7748E26DCA9}"/>
+    <hyperlink ref="L21" r:id="rId13" xr:uid="{DD6E462B-22D3-4BCE-8BEC-EE10845B77FE}"/>
+    <hyperlink ref="L17" r:id="rId14" display="https://www.arrow.com/en/products/fsm2jsmltr/te-connectivity" xr:uid="{94B52CE5-A70B-44A1-800C-359546489236}"/>
+    <hyperlink ref="L19" r:id="rId15" xr:uid="{962D090B-5AFA-4D2A-BBC2-A5C18F9637FA}"/>
     <hyperlink ref="L6" r:id="rId16" xr:uid="{6570C69E-DAF2-4C0C-B721-4156780E4DD9}"/>
+    <hyperlink ref="L3" r:id="rId17" xr:uid="{2D7342D9-B897-4BA8-9A7E-79722CCBFEDB}"/>
+    <hyperlink ref="L10" r:id="rId18" xr:uid="{9C9D096D-74A2-45B7-AFC9-26D06C091250}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Added 3.2mm drill holes to the four corners of the layout
</commit_message>
<xml_diff>
--- a/Documents/ECE_411_Bill_of_Materials.xlsx
+++ b/Documents/ECE_411_Bill_of_Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshd\Documents\Josh's\College\PSU!\ECE 411 Industry Design Processes\ece411\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE171FAE-D8ED-49EC-B1BC-D54D4BB76651}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF89CD8-1885-4551-8F8E-1A6E11C01422}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,14 +641,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1834,19 +1834,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.6" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:12" ht="20.25" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1890,7 +1890,7 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>117</v>
       </c>
       <c r="C3" s="4"/>
@@ -1917,7 +1917,7 @@
         <f>J3*A3</f>
         <v>0.16</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2186,7 +2186,7 @@
         <f t="shared" si="0"/>
         <v>0.63500000000000001</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="24" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>